<commit_message>
separate Enzyme trail 1
</commit_message>
<xml_diff>
--- a/regulondb/collection/node/TF.xlsx
+++ b/regulondb/collection/node/TF.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="730">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="736">
   <si>
     <t>ECK125140816</t>
   </si>
@@ -2214,6 +2214,30 @@
   </si>
   <si>
     <t>NAME</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>YafQ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RcsB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MazF</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BglJ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RelE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>YoeB</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2544,9 +2568,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F203"/>
+  <dimension ref="A1:F209"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
+      <selection activeCell="A203" sqref="A203"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
@@ -3413,1986 +3439,1953 @@
         <v>194</v>
       </c>
       <c r="B53" t="s">
-        <v>195</v>
-      </c>
-      <c r="E53" t="s">
-        <v>196</v>
-      </c>
-      <c r="F53" t="s">
-        <v>197</v>
+        <v>730</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B54" t="s">
-        <v>199</v>
-      </c>
-      <c r="C54" t="s">
-        <v>200</v>
-      </c>
-      <c r="D54" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="E54" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="F54" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="B55" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="C55" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="D55" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="E55" t="s">
-        <v>206</v>
-      </c>
-      <c r="F55">
-        <v>18997424</v>
+        <v>201</v>
+      </c>
+      <c r="F55" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B56" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C56" t="s">
-        <v>209</v>
+        <v>205</v>
+      </c>
+      <c r="D56" t="s">
+        <v>204</v>
       </c>
       <c r="E56" t="s">
-        <v>30</v>
+        <v>206</v>
       </c>
       <c r="F56">
-        <v>3275618</v>
+        <v>18997424</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B57" t="s">
-        <v>211</v>
+        <v>208</v>
+      </c>
+      <c r="C57" t="s">
+        <v>209</v>
       </c>
       <c r="E57" t="s">
-        <v>41</v>
+        <v>30</v>
+      </c>
+      <c r="F57">
+        <v>3275618</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B58" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E58" t="s">
-        <v>133</v>
-      </c>
-      <c r="F58" t="s">
-        <v>214</v>
+        <v>41</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B59" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="E59" t="s">
-        <v>41</v>
-      </c>
-      <c r="F59">
-        <v>2536924</v>
+        <v>133</v>
+      </c>
+      <c r="F59" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B60" t="s">
-        <v>218</v>
-      </c>
-      <c r="C60" t="s">
-        <v>219</v>
-      </c>
-      <c r="D60" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E60" t="s">
-        <v>220</v>
-      </c>
-      <c r="F60" t="s">
-        <v>221</v>
+        <v>41</v>
+      </c>
+      <c r="F60">
+        <v>2536924</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="B61" t="s">
-        <v>223</v>
+        <v>218</v>
+      </c>
+      <c r="C61" t="s">
+        <v>219</v>
+      </c>
+      <c r="D61" t="s">
+        <v>218</v>
       </c>
       <c r="E61" t="s">
-        <v>41</v>
-      </c>
-      <c r="F61">
-        <v>6357945</v>
+        <v>220</v>
+      </c>
+      <c r="F61" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B62" t="s">
-        <v>225</v>
-      </c>
-      <c r="C62" t="s">
-        <v>226</v>
-      </c>
-      <c r="D62" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E62" t="s">
-        <v>228</v>
-      </c>
-      <c r="F62" t="s">
-        <v>229</v>
+        <v>41</v>
+      </c>
+      <c r="F62">
+        <v>6357945</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="B63" t="s">
-        <v>231</v>
+        <v>225</v>
+      </c>
+      <c r="C63" t="s">
+        <v>226</v>
+      </c>
+      <c r="D63" t="s">
+        <v>227</v>
       </c>
       <c r="E63" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="F63" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B64" t="s">
-        <v>235</v>
-      </c>
-      <c r="C64" t="s">
-        <v>235</v>
-      </c>
-      <c r="D64" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="E64" t="s">
-        <v>90</v>
+        <v>232</v>
       </c>
       <c r="F64" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B65" t="s">
-        <v>239</v>
+        <v>235</v>
+      </c>
+      <c r="C65" t="s">
+        <v>235</v>
+      </c>
+      <c r="D65" t="s">
+        <v>236</v>
       </c>
       <c r="E65" t="s">
-        <v>240</v>
+        <v>90</v>
       </c>
       <c r="F65" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B66" t="s">
-        <v>243</v>
-      </c>
-      <c r="C66" t="s">
-        <v>244</v>
-      </c>
-      <c r="D66" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="E66" t="s">
-        <v>245</v>
-      </c>
-      <c r="F66">
-        <v>8034727</v>
+        <v>240</v>
+      </c>
+      <c r="F66" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B67" t="s">
-        <v>247</v>
-      </c>
-      <c r="F67" t="s">
-        <v>248</v>
+        <v>243</v>
+      </c>
+      <c r="C67" t="s">
+        <v>244</v>
+      </c>
+      <c r="D67" t="s">
+        <v>243</v>
+      </c>
+      <c r="E67" t="s">
+        <v>245</v>
+      </c>
+      <c r="F67">
+        <v>8034727</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B68" t="s">
-        <v>250</v>
-      </c>
-      <c r="E68" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="F68" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B69" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="E69" t="s">
-        <v>33</v>
-      </c>
-      <c r="F69">
-        <v>18765794</v>
+        <v>251</v>
+      </c>
+      <c r="F69" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B70" t="s">
-        <v>256</v>
-      </c>
-      <c r="C70" t="s">
-        <v>257</v>
-      </c>
-      <c r="D70" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="E70" t="s">
-        <v>75</v>
-      </c>
-      <c r="F70" t="s">
-        <v>258</v>
+        <v>33</v>
+      </c>
+      <c r="F70">
+        <v>18765794</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B71" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C71" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="D71" t="s">
-        <v>260</v>
+        <v>256</v>
+      </c>
+      <c r="E71" t="s">
+        <v>75</v>
       </c>
       <c r="F71" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="72" spans="1:6">
       <c r="A72" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B72" t="s">
-        <v>264</v>
-      </c>
-      <c r="E72" t="s">
-        <v>41</v>
+        <v>260</v>
+      </c>
+      <c r="C72" t="s">
+        <v>261</v>
+      </c>
+      <c r="D72" t="s">
+        <v>260</v>
       </c>
       <c r="F72" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="A73" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B73" t="s">
-        <v>267</v>
+        <v>264</v>
+      </c>
+      <c r="E73" t="s">
+        <v>41</v>
+      </c>
+      <c r="F73" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B74" t="s">
-        <v>269</v>
-      </c>
-      <c r="E74" t="s">
-        <v>270</v>
-      </c>
-      <c r="F74">
-        <v>12446650</v>
+        <v>731</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="B75" t="s">
-        <v>272</v>
-      </c>
-      <c r="E75" t="s">
-        <v>84</v>
-      </c>
-      <c r="F75" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="B76" t="s">
-        <v>275</v>
-      </c>
-      <c r="C76" t="s">
-        <v>275</v>
-      </c>
-      <c r="D76" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="E76" t="s">
-        <v>277</v>
-      </c>
-      <c r="F76" t="s">
-        <v>278</v>
+        <v>270</v>
+      </c>
+      <c r="F76">
+        <v>12446650</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="B77" t="s">
-        <v>280</v>
-      </c>
-      <c r="C77" t="s">
-        <v>280</v>
-      </c>
-      <c r="D77" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="E77" t="s">
-        <v>282</v>
+        <v>84</v>
       </c>
       <c r="F77" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="B78" t="s">
-        <v>285</v>
+        <v>275</v>
+      </c>
+      <c r="C78" t="s">
+        <v>275</v>
+      </c>
+      <c r="D78" t="s">
+        <v>276</v>
       </c>
       <c r="E78" t="s">
-        <v>75</v>
+        <v>277</v>
       </c>
       <c r="F78" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
     </row>
     <row r="79" spans="1:6">
       <c r="A79" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="B79" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="C79" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="D79" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="E79" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="F79" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="B80" t="s">
-        <v>293</v>
-      </c>
-      <c r="C80" t="s">
-        <v>294</v>
-      </c>
-      <c r="D80" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="E80" t="s">
-        <v>295</v>
+        <v>75</v>
       </c>
       <c r="F80" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
     </row>
     <row r="81" spans="1:6">
       <c r="A81" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="B81" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="C81" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="D81" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="E81" t="s">
-        <v>41</v>
+        <v>290</v>
       </c>
       <c r="F81" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="B82" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="C82" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="D82" t="s">
-        <v>302</v>
+        <v>293</v>
+      </c>
+      <c r="E82" t="s">
+        <v>295</v>
+      </c>
+      <c r="F82" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="B83" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="C83" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="D83" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="E83" t="s">
         <v>41</v>
       </c>
-      <c r="F83">
-        <v>8655507</v>
+      <c r="F83" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="84" spans="1:6">
       <c r="A84" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="B84" t="s">
-        <v>308</v>
-      </c>
-      <c r="E84" t="s">
-        <v>75</v>
-      </c>
-      <c r="F84">
-        <v>3062173</v>
+        <v>302</v>
+      </c>
+      <c r="C84" t="s">
+        <v>303</v>
+      </c>
+      <c r="D84" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="85" spans="1:6">
       <c r="A85" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="B85" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="C85" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="D85" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="E85" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="F85">
-        <v>3062173</v>
+        <v>8655507</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="A86" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="B86" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="E86" t="s">
-        <v>314</v>
-      </c>
-      <c r="F86" t="s">
-        <v>315</v>
+        <v>75</v>
+      </c>
+      <c r="F86">
+        <v>3062173</v>
       </c>
     </row>
     <row r="87" spans="1:6">
       <c r="A87" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="B87" t="s">
-        <v>317</v>
+        <v>310</v>
+      </c>
+      <c r="C87" t="s">
+        <v>310</v>
+      </c>
+      <c r="D87" t="s">
+        <v>311</v>
       </c>
       <c r="E87" t="s">
-        <v>318</v>
-      </c>
-      <c r="F87" t="s">
-        <v>319</v>
+        <v>75</v>
+      </c>
+      <c r="F87">
+        <v>3062173</v>
       </c>
     </row>
     <row r="88" spans="1:6">
       <c r="A88" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="B88" t="s">
-        <v>321</v>
+        <v>313</v>
+      </c>
+      <c r="E88" t="s">
+        <v>314</v>
       </c>
       <c r="F88" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
     </row>
     <row r="89" spans="1:6">
       <c r="A89" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="B89" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="E89" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="F89" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
     </row>
     <row r="90" spans="1:6">
       <c r="A90" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="B90" t="s">
-        <v>328</v>
-      </c>
-      <c r="E90" t="s">
-        <v>251</v>
-      </c>
-      <c r="F90">
-        <v>8021189</v>
+        <v>321</v>
+      </c>
+      <c r="F90" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="91" spans="1:6">
       <c r="A91" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="B91" t="s">
-        <v>330</v>
+        <v>324</v>
+      </c>
+      <c r="E91" t="s">
+        <v>325</v>
+      </c>
+      <c r="F91" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="92" spans="1:6">
       <c r="A92" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B92" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="E92" t="s">
-        <v>41</v>
+        <v>251</v>
       </c>
       <c r="F92">
-        <v>9387241</v>
+        <v>8021189</v>
       </c>
     </row>
     <row r="93" spans="1:6">
       <c r="A93" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B93" t="s">
-        <v>334</v>
-      </c>
-      <c r="E93" t="s">
-        <v>335</v>
-      </c>
-      <c r="F93" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
     </row>
     <row r="94" spans="1:6">
       <c r="A94" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="B94" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="E94" t="s">
-        <v>5</v>
-      </c>
-      <c r="F94" t="s">
-        <v>339</v>
+        <v>41</v>
+      </c>
+      <c r="F94">
+        <v>9387241</v>
       </c>
     </row>
     <row r="95" spans="1:6">
       <c r="A95" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="B95" t="s">
-        <v>341</v>
-      </c>
-      <c r="C95" t="s">
-        <v>342</v>
-      </c>
-      <c r="D95" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="E95" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="F95" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
     </row>
     <row r="96" spans="1:6">
       <c r="A96" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="B96" t="s">
-        <v>347</v>
-      </c>
-      <c r="C96" t="s">
-        <v>348</v>
-      </c>
-      <c r="D96" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="E96" t="s">
-        <v>349</v>
-      </c>
-      <c r="F96">
-        <v>14973046</v>
+        <v>5</v>
+      </c>
+      <c r="F96" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="97" spans="1:6">
       <c r="A97" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="B97" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="C97" t="s">
-        <v>352</v>
+        <v>342</v>
+      </c>
+      <c r="D97" t="s">
+        <v>343</v>
+      </c>
+      <c r="E97" t="s">
+        <v>344</v>
       </c>
       <c r="F97" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
     </row>
     <row r="98" spans="1:6">
       <c r="A98" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="B98" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="C98" t="s">
-        <v>356</v>
+        <v>348</v>
+      </c>
+      <c r="D98" t="s">
+        <v>347</v>
       </c>
       <c r="E98" t="s">
         <v>349</v>
       </c>
       <c r="F98">
-        <v>11742080</v>
+        <v>14973046</v>
       </c>
     </row>
     <row r="99" spans="1:6">
       <c r="A99" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="B99" t="s">
-        <v>358</v>
-      </c>
-      <c r="E99" t="s">
-        <v>359</v>
+        <v>351</v>
+      </c>
+      <c r="C99" t="s">
+        <v>352</v>
       </c>
       <c r="F99" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
     </row>
     <row r="100" spans="1:6">
       <c r="A100" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="B100" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="C100" t="s">
-        <v>363</v>
-      </c>
-      <c r="D100" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="E100" t="s">
-        <v>364</v>
-      </c>
-      <c r="F100" t="s">
-        <v>365</v>
+        <v>349</v>
+      </c>
+      <c r="F100">
+        <v>11742080</v>
       </c>
     </row>
     <row r="101" spans="1:6">
       <c r="A101" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
       <c r="B101" t="s">
-        <v>367</v>
-      </c>
-      <c r="C101" t="s">
-        <v>367</v>
-      </c>
-      <c r="D101" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="E101" t="s">
-        <v>41</v>
+        <v>359</v>
       </c>
       <c r="F101" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
     </row>
     <row r="102" spans="1:6">
       <c r="A102" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
       <c r="B102" t="s">
-        <v>371</v>
+        <v>362</v>
+      </c>
+      <c r="C102" t="s">
+        <v>363</v>
+      </c>
+      <c r="D102" t="s">
+        <v>362</v>
       </c>
       <c r="E102" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="F102" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
     </row>
     <row r="103" spans="1:6">
       <c r="A103" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="B103" t="s">
-        <v>375</v>
+        <v>367</v>
+      </c>
+      <c r="C103" t="s">
+        <v>367</v>
+      </c>
+      <c r="D103" t="s">
+        <v>368</v>
       </c>
       <c r="E103" t="s">
-        <v>376</v>
+        <v>41</v>
       </c>
       <c r="F103" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
     </row>
     <row r="104" spans="1:6">
       <c r="A104" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="B104" t="s">
-        <v>379</v>
-      </c>
-      <c r="C104" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
       <c r="E104" t="s">
-        <v>41</v>
+        <v>372</v>
+      </c>
+      <c r="F104" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="105" spans="1:6">
       <c r="A105" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="B105" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="E105" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="F105" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
     </row>
     <row r="106" spans="1:6">
       <c r="A106" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="B106" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="C106" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="E106" t="s">
-        <v>228</v>
-      </c>
-      <c r="F106" t="s">
-        <v>388</v>
+        <v>41</v>
       </c>
     </row>
     <row r="107" spans="1:6">
       <c r="A107" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="B107" t="s">
-        <v>390</v>
-      </c>
-      <c r="C107" t="s">
-        <v>390</v>
-      </c>
-      <c r="D107" t="s">
-        <v>391</v>
+        <v>382</v>
       </c>
       <c r="E107" t="s">
-        <v>201</v>
+        <v>383</v>
       </c>
       <c r="F107" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
     </row>
     <row r="108" spans="1:6">
       <c r="A108" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="B108" t="s">
-        <v>394</v>
+        <v>386</v>
+      </c>
+      <c r="C108" t="s">
+        <v>387</v>
       </c>
       <c r="E108" t="s">
-        <v>41</v>
-      </c>
-      <c r="F108">
-        <v>6350602</v>
+        <v>228</v>
+      </c>
+      <c r="F108" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="109" spans="1:6">
       <c r="A109" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="B109" t="s">
-        <v>396</v>
+        <v>390</v>
+      </c>
+      <c r="C109" t="s">
+        <v>390</v>
+      </c>
+      <c r="D109" t="s">
+        <v>391</v>
       </c>
       <c r="E109" t="s">
-        <v>397</v>
+        <v>201</v>
       </c>
       <c r="F109" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
     </row>
     <row r="110" spans="1:6">
       <c r="A110" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="B110" t="s">
-        <v>400</v>
-      </c>
-      <c r="C110" t="s">
-        <v>401</v>
-      </c>
-      <c r="D110" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="E110" t="s">
-        <v>251</v>
-      </c>
-      <c r="F110" t="s">
-        <v>403</v>
+        <v>41</v>
+      </c>
+      <c r="F110">
+        <v>6350602</v>
       </c>
     </row>
     <row r="111" spans="1:6">
       <c r="A111" t="s">
-        <v>404</v>
+        <v>395</v>
       </c>
       <c r="B111" t="s">
-        <v>405</v>
+        <v>396</v>
       </c>
       <c r="E111" t="s">
-        <v>41</v>
+        <v>397</v>
       </c>
       <c r="F111" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
     </row>
     <row r="112" spans="1:6">
       <c r="A112" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="B112" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="C112" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="D112" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="E112" t="s">
         <v>251</v>
       </c>
       <c r="F112" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
     </row>
     <row r="113" spans="1:6">
       <c r="A113" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="B113" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="E113" t="s">
-        <v>125</v>
+        <v>41</v>
       </c>
       <c r="F113" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
     </row>
     <row r="114" spans="1:6">
       <c r="A114" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="B114" t="s">
-        <v>415</v>
+        <v>408</v>
+      </c>
+      <c r="C114" t="s">
+        <v>408</v>
+      </c>
+      <c r="D114" t="s">
+        <v>409</v>
+      </c>
+      <c r="E114" t="s">
+        <v>251</v>
+      </c>
+      <c r="F114" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="115" spans="1:6">
       <c r="A115" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="B115" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="E115" t="s">
-        <v>41</v>
+        <v>125</v>
+      </c>
+      <c r="F115" t="s">
+        <v>413</v>
       </c>
     </row>
     <row r="116" spans="1:6">
       <c r="A116" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="B116" t="s">
-        <v>419</v>
-      </c>
-      <c r="E116" t="s">
-        <v>420</v>
-      </c>
-      <c r="F116" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
     </row>
     <row r="117" spans="1:6">
       <c r="A117" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="B117" t="s">
-        <v>423</v>
-      </c>
-      <c r="C117" t="s">
-        <v>424</v>
-      </c>
-      <c r="E117" t="s">
-        <v>425</v>
-      </c>
-      <c r="F117" t="s">
-        <v>426</v>
+        <v>732</v>
       </c>
     </row>
     <row r="118" spans="1:6">
       <c r="A118" t="s">
-        <v>427</v>
+        <v>416</v>
       </c>
       <c r="B118" t="s">
-        <v>428</v>
-      </c>
-      <c r="C118" t="s">
-        <v>429</v>
-      </c>
-      <c r="D118" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
       <c r="E118" t="s">
-        <v>228</v>
-      </c>
-      <c r="F118" t="s">
-        <v>430</v>
+        <v>41</v>
       </c>
     </row>
     <row r="119" spans="1:6">
       <c r="A119" t="s">
-        <v>431</v>
+        <v>418</v>
       </c>
       <c r="B119" t="s">
-        <v>432</v>
-      </c>
-      <c r="C119" t="s">
-        <v>433</v>
-      </c>
-      <c r="D119" t="s">
-        <v>432</v>
+        <v>419</v>
       </c>
       <c r="E119" t="s">
-        <v>23</v>
+        <v>420</v>
       </c>
       <c r="F119" t="s">
-        <v>434</v>
+        <v>421</v>
       </c>
     </row>
     <row r="120" spans="1:6">
       <c r="A120" t="s">
-        <v>435</v>
+        <v>422</v>
       </c>
       <c r="B120" t="s">
-        <v>436</v>
+        <v>423</v>
       </c>
       <c r="C120" t="s">
-        <v>437</v>
-      </c>
-      <c r="D120" t="s">
-        <v>436</v>
+        <v>424</v>
       </c>
       <c r="E120" t="s">
-        <v>75</v>
+        <v>425</v>
       </c>
       <c r="F120" t="s">
-        <v>438</v>
+        <v>426</v>
       </c>
     </row>
     <row r="121" spans="1:6">
       <c r="A121" t="s">
-        <v>439</v>
+        <v>427</v>
       </c>
       <c r="B121" t="s">
-        <v>440</v>
+        <v>428</v>
       </c>
       <c r="C121" t="s">
-        <v>440</v>
+        <v>429</v>
       </c>
       <c r="D121" t="s">
-        <v>441</v>
+        <v>428</v>
       </c>
       <c r="E121" t="s">
-        <v>442</v>
+        <v>228</v>
       </c>
       <c r="F121" t="s">
-        <v>443</v>
+        <v>430</v>
       </c>
     </row>
     <row r="122" spans="1:6">
       <c r="A122" t="s">
-        <v>444</v>
+        <v>431</v>
       </c>
       <c r="B122" t="s">
-        <v>445</v>
+        <v>432</v>
+      </c>
+      <c r="C122" t="s">
+        <v>433</v>
+      </c>
+      <c r="D122" t="s">
+        <v>432</v>
       </c>
       <c r="E122" t="s">
-        <v>446</v>
+        <v>23</v>
       </c>
       <c r="F122" t="s">
-        <v>447</v>
+        <v>434</v>
       </c>
     </row>
     <row r="123" spans="1:6">
       <c r="A123" t="s">
-        <v>448</v>
+        <v>435</v>
       </c>
       <c r="B123" t="s">
-        <v>449</v>
+        <v>436</v>
+      </c>
+      <c r="C123" t="s">
+        <v>437</v>
+      </c>
+      <c r="D123" t="s">
+        <v>436</v>
       </c>
       <c r="E123" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
       <c r="F123" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
     </row>
     <row r="124" spans="1:6">
       <c r="A124" t="s">
-        <v>451</v>
+        <v>439</v>
       </c>
       <c r="B124" t="s">
-        <v>452</v>
+        <v>440</v>
       </c>
       <c r="C124" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
       <c r="D124" t="s">
-        <v>452</v>
+        <v>441</v>
       </c>
       <c r="E124" t="s">
-        <v>454</v>
+        <v>442</v>
       </c>
       <c r="F124" t="s">
-        <v>455</v>
+        <v>443</v>
       </c>
     </row>
     <row r="125" spans="1:6">
       <c r="A125" t="s">
-        <v>456</v>
+        <v>444</v>
       </c>
       <c r="B125" t="s">
-        <v>457</v>
-      </c>
-      <c r="C125" t="s">
-        <v>458</v>
-      </c>
-      <c r="D125" t="s">
-        <v>457</v>
+        <v>445</v>
       </c>
       <c r="E125" t="s">
-        <v>459</v>
+        <v>446</v>
       </c>
       <c r="F125" t="s">
-        <v>460</v>
+        <v>447</v>
       </c>
     </row>
     <row r="126" spans="1:6">
       <c r="A126" t="s">
-        <v>461</v>
+        <v>448</v>
       </c>
       <c r="B126" t="s">
-        <v>462</v>
-      </c>
-      <c r="C126" t="s">
-        <v>462</v>
-      </c>
-      <c r="D126" t="s">
-        <v>463</v>
+        <v>449</v>
       </c>
       <c r="E126" t="s">
-        <v>251</v>
+        <v>23</v>
       </c>
       <c r="F126" t="s">
-        <v>464</v>
+        <v>450</v>
       </c>
     </row>
     <row r="127" spans="1:6">
       <c r="A127" t="s">
-        <v>465</v>
+        <v>451</v>
       </c>
       <c r="B127" t="s">
-        <v>466</v>
+        <v>452</v>
+      </c>
+      <c r="C127" t="s">
+        <v>453</v>
+      </c>
+      <c r="D127" t="s">
+        <v>452</v>
       </c>
       <c r="E127" t="s">
-        <v>467</v>
+        <v>454</v>
       </c>
       <c r="F127" t="s">
-        <v>468</v>
+        <v>455</v>
       </c>
     </row>
     <row r="128" spans="1:6">
       <c r="A128" t="s">
-        <v>469</v>
+        <v>456</v>
       </c>
       <c r="B128" t="s">
-        <v>470</v>
+        <v>457</v>
+      </c>
+      <c r="C128" t="s">
+        <v>458</v>
+      </c>
+      <c r="D128" t="s">
+        <v>457</v>
       </c>
       <c r="E128" t="s">
-        <v>41</v>
+        <v>459</v>
       </c>
       <c r="F128" t="s">
-        <v>471</v>
+        <v>460</v>
       </c>
     </row>
     <row r="129" spans="1:6">
       <c r="A129" t="s">
-        <v>472</v>
+        <v>461</v>
       </c>
       <c r="B129" t="s">
-        <v>473</v>
+        <v>462</v>
       </c>
       <c r="C129" t="s">
-        <v>473</v>
+        <v>462</v>
       </c>
       <c r="D129" t="s">
-        <v>474</v>
+        <v>463</v>
       </c>
       <c r="E129" t="s">
-        <v>90</v>
-      </c>
-      <c r="F129">
-        <v>18723630</v>
+        <v>251</v>
+      </c>
+      <c r="F129" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="130" spans="1:6">
       <c r="A130" t="s">
-        <v>475</v>
+        <v>465</v>
       </c>
       <c r="B130" t="s">
-        <v>476</v>
+        <v>466</v>
       </c>
       <c r="E130" t="s">
-        <v>477</v>
+        <v>467</v>
       </c>
       <c r="F130" t="s">
-        <v>478</v>
+        <v>468</v>
       </c>
     </row>
     <row r="131" spans="1:6">
       <c r="A131" t="s">
-        <v>479</v>
+        <v>469</v>
       </c>
       <c r="B131" t="s">
-        <v>480</v>
+        <v>470</v>
       </c>
       <c r="E131" t="s">
-        <v>481</v>
+        <v>41</v>
       </c>
       <c r="F131" t="s">
-        <v>482</v>
+        <v>471</v>
       </c>
     </row>
     <row r="132" spans="1:6">
       <c r="A132" t="s">
-        <v>483</v>
+        <v>472</v>
       </c>
       <c r="B132" t="s">
-        <v>484</v>
+        <v>473</v>
       </c>
       <c r="C132" t="s">
-        <v>484</v>
+        <v>473</v>
       </c>
       <c r="D132" t="s">
-        <v>485</v>
+        <v>474</v>
       </c>
       <c r="E132" t="s">
-        <v>251</v>
-      </c>
-      <c r="F132" t="s">
-        <v>486</v>
+        <v>90</v>
+      </c>
+      <c r="F132">
+        <v>18723630</v>
       </c>
     </row>
     <row r="133" spans="1:6">
       <c r="A133" t="s">
-        <v>487</v>
+        <v>475</v>
       </c>
       <c r="B133" t="s">
-        <v>488</v>
-      </c>
-      <c r="C133" t="s">
-        <v>488</v>
-      </c>
-      <c r="D133" t="s">
-        <v>489</v>
+        <v>476</v>
       </c>
       <c r="E133" t="s">
-        <v>245</v>
-      </c>
-      <c r="F133">
-        <v>12897000</v>
+        <v>477</v>
+      </c>
+      <c r="F133" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="134" spans="1:6">
       <c r="A134" t="s">
-        <v>490</v>
+        <v>479</v>
       </c>
       <c r="B134" t="s">
-        <v>491</v>
-      </c>
-      <c r="C134" t="s">
-        <v>492</v>
-      </c>
-      <c r="D134" t="s">
-        <v>491</v>
+        <v>480</v>
       </c>
       <c r="E134" t="s">
-        <v>157</v>
+        <v>481</v>
       </c>
       <c r="F134" t="s">
-        <v>493</v>
+        <v>482</v>
       </c>
     </row>
     <row r="135" spans="1:6">
       <c r="A135" t="s">
-        <v>494</v>
+        <v>483</v>
       </c>
       <c r="B135" t="s">
-        <v>495</v>
+        <v>484</v>
       </c>
       <c r="C135" t="s">
-        <v>496</v>
+        <v>484</v>
       </c>
       <c r="D135" t="s">
-        <v>495</v>
+        <v>485</v>
       </c>
       <c r="E135" t="s">
-        <v>157</v>
+        <v>251</v>
       </c>
       <c r="F135" t="s">
-        <v>497</v>
+        <v>486</v>
       </c>
     </row>
     <row r="136" spans="1:6">
       <c r="A136" t="s">
-        <v>498</v>
+        <v>487</v>
       </c>
       <c r="B136" t="s">
-        <v>499</v>
+        <v>488</v>
+      </c>
+      <c r="C136" t="s">
+        <v>488</v>
+      </c>
+      <c r="D136" t="s">
+        <v>489</v>
       </c>
       <c r="E136" t="s">
-        <v>133</v>
-      </c>
-      <c r="F136" t="s">
-        <v>500</v>
+        <v>245</v>
+      </c>
+      <c r="F136">
+        <v>12897000</v>
       </c>
     </row>
     <row r="137" spans="1:6">
       <c r="A137" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
       <c r="B137" t="s">
-        <v>502</v>
+        <v>491</v>
       </c>
       <c r="C137" t="s">
-        <v>503</v>
+        <v>492</v>
       </c>
       <c r="D137" t="s">
-        <v>502</v>
+        <v>491</v>
       </c>
       <c r="E137" t="s">
-        <v>364</v>
+        <v>157</v>
       </c>
       <c r="F137" t="s">
-        <v>504</v>
+        <v>493</v>
       </c>
     </row>
     <row r="138" spans="1:6">
       <c r="A138" t="s">
-        <v>505</v>
+        <v>494</v>
       </c>
       <c r="B138" t="s">
-        <v>506</v>
+        <v>495</v>
       </c>
       <c r="C138" t="s">
-        <v>507</v>
+        <v>496</v>
       </c>
       <c r="D138" t="s">
-        <v>506</v>
+        <v>495</v>
       </c>
       <c r="E138" t="s">
-        <v>251</v>
-      </c>
-      <c r="F138">
-        <v>10787413</v>
+        <v>157</v>
+      </c>
+      <c r="F138" t="s">
+        <v>497</v>
       </c>
     </row>
     <row r="139" spans="1:6">
       <c r="A139" t="s">
-        <v>508</v>
+        <v>498</v>
       </c>
       <c r="B139" t="s">
-        <v>509</v>
+        <v>499</v>
       </c>
       <c r="E139" t="s">
-        <v>510</v>
+        <v>133</v>
       </c>
       <c r="F139" t="s">
-        <v>511</v>
+        <v>500</v>
       </c>
     </row>
     <row r="140" spans="1:6">
       <c r="A140" t="s">
-        <v>512</v>
+        <v>501</v>
       </c>
       <c r="B140" t="s">
-        <v>513</v>
+        <v>502</v>
       </c>
       <c r="C140" t="s">
-        <v>514</v>
+        <v>503</v>
+      </c>
+      <c r="D140" t="s">
+        <v>502</v>
       </c>
       <c r="E140" t="s">
-        <v>157</v>
-      </c>
-      <c r="F140">
-        <v>17496099</v>
+        <v>364</v>
+      </c>
+      <c r="F140" t="s">
+        <v>504</v>
       </c>
     </row>
     <row r="141" spans="1:6">
       <c r="A141" t="s">
-        <v>515</v>
+        <v>505</v>
       </c>
       <c r="B141" t="s">
-        <v>516</v>
+        <v>506</v>
       </c>
       <c r="C141" t="s">
-        <v>517</v>
+        <v>507</v>
       </c>
       <c r="D141" t="s">
-        <v>518</v>
+        <v>506</v>
       </c>
       <c r="E141" t="s">
-        <v>519</v>
-      </c>
-      <c r="F141" t="s">
-        <v>520</v>
+        <v>251</v>
+      </c>
+      <c r="F141">
+        <v>10787413</v>
       </c>
     </row>
     <row r="142" spans="1:6">
       <c r="A142" t="s">
-        <v>521</v>
+        <v>508</v>
       </c>
       <c r="B142" t="s">
-        <v>522</v>
-      </c>
-      <c r="C142" t="s">
-        <v>523</v>
-      </c>
-      <c r="D142" t="s">
-        <v>522</v>
+        <v>509</v>
       </c>
       <c r="E142" t="s">
-        <v>228</v>
+        <v>510</v>
       </c>
       <c r="F142" t="s">
-        <v>524</v>
+        <v>511</v>
       </c>
     </row>
     <row r="143" spans="1:6">
       <c r="A143" t="s">
-        <v>525</v>
+        <v>512</v>
       </c>
       <c r="B143" t="s">
-        <v>526</v>
+        <v>513</v>
       </c>
       <c r="C143" t="s">
-        <v>527</v>
-      </c>
-      <c r="D143" t="s">
-        <v>526</v>
+        <v>514</v>
       </c>
       <c r="E143" t="s">
         <v>157</v>
       </c>
-      <c r="F143" t="s">
-        <v>528</v>
+      <c r="F143">
+        <v>17496099</v>
       </c>
     </row>
     <row r="144" spans="1:6">
       <c r="A144" t="s">
-        <v>529</v>
+        <v>515</v>
       </c>
       <c r="B144" t="s">
-        <v>530</v>
+        <v>516</v>
+      </c>
+      <c r="C144" t="s">
+        <v>517</v>
+      </c>
+      <c r="D144" t="s">
+        <v>518</v>
       </c>
       <c r="E144" t="s">
-        <v>206</v>
+        <v>519</v>
       </c>
       <c r="F144" t="s">
-        <v>531</v>
+        <v>520</v>
       </c>
     </row>
     <row r="145" spans="1:6">
       <c r="A145" t="s">
-        <v>532</v>
+        <v>521</v>
       </c>
       <c r="B145" t="s">
-        <v>533</v>
+        <v>522</v>
+      </c>
+      <c r="C145" t="s">
+        <v>523</v>
+      </c>
+      <c r="D145" t="s">
+        <v>522</v>
       </c>
       <c r="E145" t="s">
-        <v>30</v>
-      </c>
-      <c r="F145">
-        <v>10766858</v>
+        <v>228</v>
+      </c>
+      <c r="F145" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="146" spans="1:6">
       <c r="A146" t="s">
-        <v>534</v>
+        <v>525</v>
       </c>
       <c r="B146" t="s">
-        <v>535</v>
+        <v>526</v>
       </c>
       <c r="C146" t="s">
-        <v>535</v>
+        <v>527</v>
       </c>
       <c r="D146" t="s">
-        <v>536</v>
+        <v>526</v>
       </c>
       <c r="E146" t="s">
-        <v>537</v>
+        <v>157</v>
       </c>
       <c r="F146" t="s">
-        <v>538</v>
+        <v>528</v>
       </c>
     </row>
     <row r="147" spans="1:6">
       <c r="A147" t="s">
-        <v>539</v>
+        <v>529</v>
       </c>
       <c r="B147" t="s">
-        <v>540</v>
-      </c>
-      <c r="F147">
-        <v>14741201</v>
+        <v>530</v>
+      </c>
+      <c r="E147" t="s">
+        <v>206</v>
+      </c>
+      <c r="F147" t="s">
+        <v>531</v>
       </c>
     </row>
     <row r="148" spans="1:6">
       <c r="A148" t="s">
-        <v>541</v>
+        <v>532</v>
       </c>
       <c r="B148" t="s">
-        <v>542</v>
+        <v>533</v>
       </c>
       <c r="E148" t="s">
-        <v>543</v>
-      </c>
-      <c r="F148" t="s">
-        <v>544</v>
+        <v>30</v>
+      </c>
+      <c r="F148">
+        <v>10766858</v>
       </c>
     </row>
     <row r="149" spans="1:6">
       <c r="A149" t="s">
-        <v>545</v>
+        <v>534</v>
       </c>
       <c r="B149" t="s">
-        <v>546</v>
+        <v>535</v>
       </c>
       <c r="C149" t="s">
-        <v>547</v>
+        <v>535</v>
       </c>
       <c r="D149" t="s">
-        <v>546</v>
+        <v>536</v>
+      </c>
+      <c r="E149" t="s">
+        <v>537</v>
+      </c>
+      <c r="F149" t="s">
+        <v>538</v>
       </c>
     </row>
     <row r="150" spans="1:6">
       <c r="A150" t="s">
-        <v>548</v>
+        <v>539</v>
       </c>
       <c r="B150" t="s">
-        <v>549</v>
-      </c>
-      <c r="C150" t="s">
-        <v>550</v>
-      </c>
-      <c r="D150" t="s">
-        <v>549</v>
-      </c>
-      <c r="E150" t="s">
-        <v>157</v>
-      </c>
-      <c r="F150" t="s">
-        <v>551</v>
+        <v>540</v>
+      </c>
+      <c r="F150">
+        <v>14741201</v>
       </c>
     </row>
     <row r="151" spans="1:6">
       <c r="A151" t="s">
-        <v>552</v>
+        <v>541</v>
       </c>
       <c r="B151" t="s">
-        <v>553</v>
-      </c>
-      <c r="C151" t="s">
-        <v>554</v>
+        <v>542</v>
       </c>
       <c r="E151" t="s">
-        <v>349</v>
-      </c>
-      <c r="F151">
-        <v>15805526</v>
+        <v>543</v>
+      </c>
+      <c r="F151" t="s">
+        <v>544</v>
       </c>
     </row>
     <row r="152" spans="1:6">
       <c r="A152" t="s">
-        <v>555</v>
+        <v>545</v>
       </c>
       <c r="B152" t="s">
-        <v>556</v>
+        <v>546</v>
+      </c>
+      <c r="C152" t="s">
+        <v>547</v>
+      </c>
+      <c r="D152" t="s">
+        <v>546</v>
       </c>
     </row>
     <row r="153" spans="1:6">
       <c r="A153" t="s">
-        <v>557</v>
+        <v>548</v>
       </c>
       <c r="B153" t="s">
-        <v>558</v>
+        <v>549</v>
       </c>
       <c r="C153" t="s">
-        <v>559</v>
+        <v>550</v>
       </c>
       <c r="D153" t="s">
-        <v>558</v>
+        <v>549</v>
       </c>
       <c r="E153" t="s">
-        <v>228</v>
+        <v>157</v>
       </c>
       <c r="F153" t="s">
-        <v>560</v>
+        <v>551</v>
       </c>
     </row>
     <row r="154" spans="1:6">
       <c r="A154" t="s">
-        <v>561</v>
+        <v>552</v>
       </c>
       <c r="B154" t="s">
-        <v>562</v>
+        <v>553</v>
+      </c>
+      <c r="C154" t="s">
+        <v>554</v>
+      </c>
+      <c r="E154" t="s">
+        <v>349</v>
+      </c>
+      <c r="F154">
+        <v>15805526</v>
       </c>
     </row>
     <row r="155" spans="1:6">
       <c r="A155" t="s">
-        <v>563</v>
+        <v>555</v>
       </c>
       <c r="B155" t="s">
-        <v>564</v>
-      </c>
-      <c r="E155" t="s">
-        <v>481</v>
-      </c>
-      <c r="F155" t="s">
-        <v>565</v>
+        <v>556</v>
       </c>
     </row>
     <row r="156" spans="1:6">
       <c r="A156" t="s">
-        <v>566</v>
+        <v>557</v>
       </c>
       <c r="B156" t="s">
-        <v>567</v>
+        <v>558</v>
       </c>
       <c r="C156" t="s">
-        <v>568</v>
+        <v>559</v>
       </c>
       <c r="D156" t="s">
-        <v>567</v>
+        <v>558</v>
       </c>
       <c r="E156" t="s">
-        <v>152</v>
+        <v>228</v>
       </c>
       <c r="F156" t="s">
-        <v>569</v>
+        <v>560</v>
       </c>
     </row>
     <row r="157" spans="1:6">
       <c r="A157" t="s">
-        <v>570</v>
+        <v>561</v>
       </c>
       <c r="B157" t="s">
-        <v>571</v>
-      </c>
-      <c r="C157" t="s">
-        <v>571</v>
-      </c>
-      <c r="D157" t="s">
-        <v>572</v>
-      </c>
-      <c r="E157" t="s">
-        <v>41</v>
-      </c>
-      <c r="F157" t="s">
-        <v>573</v>
+        <v>562</v>
       </c>
     </row>
     <row r="158" spans="1:6">
       <c r="A158" t="s">
-        <v>574</v>
+        <v>563</v>
       </c>
       <c r="B158" t="s">
-        <v>575</v>
+        <v>564</v>
       </c>
       <c r="E158" t="s">
-        <v>576</v>
+        <v>481</v>
       </c>
       <c r="F158" t="s">
-        <v>577</v>
+        <v>565</v>
       </c>
     </row>
     <row r="159" spans="1:6">
       <c r="A159" t="s">
-        <v>578</v>
+        <v>566</v>
       </c>
       <c r="B159" t="s">
-        <v>579</v>
+        <v>567</v>
+      </c>
+      <c r="C159" t="s">
+        <v>568</v>
+      </c>
+      <c r="D159" t="s">
+        <v>567</v>
       </c>
       <c r="E159" t="s">
-        <v>97</v>
+        <v>152</v>
       </c>
       <c r="F159" t="s">
-        <v>580</v>
+        <v>569</v>
       </c>
     </row>
     <row r="160" spans="1:6">
       <c r="A160" t="s">
-        <v>581</v>
+        <v>570</v>
       </c>
       <c r="B160" t="s">
-        <v>582</v>
+        <v>571</v>
       </c>
       <c r="C160" t="s">
-        <v>582</v>
+        <v>571</v>
       </c>
       <c r="D160" t="s">
-        <v>583</v>
+        <v>572</v>
       </c>
       <c r="E160" t="s">
-        <v>84</v>
+        <v>41</v>
       </c>
       <c r="F160" t="s">
-        <v>584</v>
+        <v>573</v>
       </c>
     </row>
     <row r="161" spans="1:6">
       <c r="A161" t="s">
-        <v>585</v>
+        <v>574</v>
       </c>
       <c r="B161" t="s">
-        <v>586</v>
+        <v>575</v>
+      </c>
+      <c r="E161" t="s">
+        <v>576</v>
+      </c>
+      <c r="F161" t="s">
+        <v>577</v>
       </c>
     </row>
     <row r="162" spans="1:6">
       <c r="A162" t="s">
-        <v>587</v>
+        <v>578</v>
       </c>
       <c r="B162" t="s">
-        <v>588</v>
+        <v>579</v>
+      </c>
+      <c r="E162" t="s">
+        <v>97</v>
+      </c>
+      <c r="F162" t="s">
+        <v>580</v>
       </c>
     </row>
     <row r="163" spans="1:6">
       <c r="A163" t="s">
-        <v>589</v>
+        <v>581</v>
       </c>
       <c r="B163" t="s">
-        <v>590</v>
+        <v>582</v>
+      </c>
+      <c r="C163" t="s">
+        <v>582</v>
+      </c>
+      <c r="D163" t="s">
+        <v>583</v>
       </c>
       <c r="E163" t="s">
-        <v>591</v>
-      </c>
-      <c r="F163">
-        <v>20952573</v>
+        <v>84</v>
+      </c>
+      <c r="F163" t="s">
+        <v>584</v>
       </c>
     </row>
     <row r="164" spans="1:6">
       <c r="A164" t="s">
-        <v>592</v>
+        <v>585</v>
       </c>
       <c r="B164" t="s">
-        <v>593</v>
-      </c>
-      <c r="E164" t="s">
-        <v>251</v>
-      </c>
-      <c r="F164">
-        <v>10501926</v>
+        <v>586</v>
       </c>
     </row>
     <row r="165" spans="1:6">
       <c r="A165" t="s">
-        <v>594</v>
+        <v>587</v>
       </c>
       <c r="B165" t="s">
-        <v>595</v>
+        <v>588</v>
       </c>
     </row>
     <row r="166" spans="1:6">
       <c r="A166" t="s">
-        <v>596</v>
+        <v>589</v>
       </c>
       <c r="B166" t="s">
-        <v>597</v>
-      </c>
-      <c r="C166" t="s">
-        <v>598</v>
-      </c>
-      <c r="E166" t="s">
-        <v>90</v>
-      </c>
-      <c r="F166" t="s">
-        <v>599</v>
+        <v>733</v>
       </c>
     </row>
     <row r="167" spans="1:6">
       <c r="A167" t="s">
-        <v>600</v>
+        <v>589</v>
       </c>
       <c r="B167" t="s">
-        <v>601</v>
-      </c>
-      <c r="C167" t="s">
-        <v>602</v>
+        <v>590</v>
       </c>
       <c r="E167" t="s">
-        <v>314</v>
-      </c>
-      <c r="F167" t="s">
-        <v>603</v>
+        <v>591</v>
+      </c>
+      <c r="F167">
+        <v>20952573</v>
       </c>
     </row>
     <row r="168" spans="1:6">
       <c r="A168" t="s">
-        <v>604</v>
+        <v>592</v>
       </c>
       <c r="B168" t="s">
-        <v>605</v>
+        <v>593</v>
       </c>
       <c r="E168" t="s">
-        <v>41</v>
-      </c>
-      <c r="F168" t="s">
-        <v>606</v>
+        <v>251</v>
+      </c>
+      <c r="F168">
+        <v>10501926</v>
       </c>
     </row>
     <row r="169" spans="1:6">
       <c r="A169" t="s">
-        <v>607</v>
+        <v>594</v>
       </c>
       <c r="B169" t="s">
-        <v>608</v>
-      </c>
-      <c r="C169" t="s">
-        <v>609</v>
-      </c>
-      <c r="D169" t="s">
-        <v>608</v>
-      </c>
-      <c r="E169" t="s">
-        <v>33</v>
-      </c>
-      <c r="F169" t="s">
-        <v>610</v>
+        <v>734</v>
       </c>
     </row>
     <row r="170" spans="1:6">
       <c r="A170" t="s">
-        <v>611</v>
+        <v>594</v>
       </c>
       <c r="B170" t="s">
-        <v>612</v>
-      </c>
-      <c r="E170" t="s">
-        <v>13</v>
-      </c>
-      <c r="F170">
-        <v>9738023</v>
+        <v>595</v>
       </c>
     </row>
     <row r="171" spans="1:6">
       <c r="A171" t="s">
-        <v>613</v>
+        <v>596</v>
       </c>
       <c r="B171" t="s">
-        <v>614</v>
+        <v>597</v>
       </c>
       <c r="C171" t="s">
-        <v>614</v>
-      </c>
-      <c r="D171" t="s">
-        <v>615</v>
+        <v>598</v>
       </c>
       <c r="E171" t="s">
-        <v>616</v>
+        <v>90</v>
       </c>
       <c r="F171" t="s">
-        <v>617</v>
+        <v>599</v>
       </c>
     </row>
     <row r="172" spans="1:6">
       <c r="A172" t="s">
-        <v>618</v>
+        <v>600</v>
       </c>
       <c r="B172" t="s">
-        <v>619</v>
+        <v>601</v>
+      </c>
+      <c r="C172" t="s">
+        <v>602</v>
       </c>
       <c r="E172" t="s">
-        <v>41</v>
+        <v>314</v>
+      </c>
+      <c r="F172" t="s">
+        <v>603</v>
       </c>
     </row>
     <row r="173" spans="1:6">
       <c r="A173" t="s">
-        <v>620</v>
+        <v>604</v>
       </c>
       <c r="B173" t="s">
-        <v>621</v>
+        <v>605</v>
       </c>
       <c r="E173" t="s">
-        <v>33</v>
-      </c>
-      <c r="F173">
-        <v>15522088</v>
+        <v>41</v>
+      </c>
+      <c r="F173" t="s">
+        <v>606</v>
       </c>
     </row>
     <row r="174" spans="1:6">
       <c r="A174" t="s">
-        <v>622</v>
+        <v>607</v>
       </c>
       <c r="B174" t="s">
-        <v>623</v>
+        <v>608</v>
+      </c>
+      <c r="C174" t="s">
+        <v>609</v>
+      </c>
+      <c r="D174" t="s">
+        <v>608</v>
       </c>
       <c r="E174" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F174" t="s">
-        <v>624</v>
+        <v>610</v>
       </c>
     </row>
     <row r="175" spans="1:6">
       <c r="A175" t="s">
-        <v>625</v>
+        <v>611</v>
       </c>
       <c r="B175" t="s">
-        <v>626</v>
-      </c>
-      <c r="C175" t="s">
-        <v>627</v>
-      </c>
-      <c r="D175" t="s">
-        <v>628</v>
+        <v>612</v>
       </c>
       <c r="E175" t="s">
-        <v>206</v>
-      </c>
-      <c r="F175" t="s">
-        <v>629</v>
+        <v>13</v>
+      </c>
+      <c r="F175">
+        <v>9738023</v>
       </c>
     </row>
     <row r="176" spans="1:6">
       <c r="A176" t="s">
-        <v>630</v>
+        <v>613</v>
       </c>
       <c r="B176" t="s">
-        <v>631</v>
+        <v>614</v>
+      </c>
+      <c r="C176" t="s">
+        <v>614</v>
+      </c>
+      <c r="D176" t="s">
+        <v>615</v>
       </c>
       <c r="E176" t="s">
-        <v>41</v>
+        <v>616</v>
       </c>
       <c r="F176" t="s">
-        <v>632</v>
+        <v>617</v>
       </c>
     </row>
     <row r="177" spans="1:6">
       <c r="A177" t="s">
-        <v>633</v>
+        <v>618</v>
       </c>
       <c r="B177" t="s">
-        <v>634</v>
+        <v>619</v>
       </c>
       <c r="E177" t="s">
         <v>41</v>
@@ -5400,422 +5393,503 @@
     </row>
     <row r="178" spans="1:6">
       <c r="A178" t="s">
-        <v>635</v>
+        <v>620</v>
       </c>
       <c r="B178" t="s">
-        <v>636</v>
+        <v>621</v>
       </c>
       <c r="E178" t="s">
-        <v>41</v>
-      </c>
-      <c r="F178" t="s">
-        <v>637</v>
+        <v>33</v>
+      </c>
+      <c r="F178">
+        <v>15522088</v>
       </c>
     </row>
     <row r="179" spans="1:6">
       <c r="A179" t="s">
-        <v>638</v>
+        <v>622</v>
       </c>
       <c r="B179" t="s">
-        <v>639</v>
+        <v>623</v>
       </c>
       <c r="E179" t="s">
         <v>41</v>
       </c>
       <c r="F179" t="s">
-        <v>640</v>
+        <v>624</v>
       </c>
     </row>
     <row r="180" spans="1:6">
       <c r="A180" t="s">
-        <v>641</v>
+        <v>625</v>
       </c>
       <c r="B180" t="s">
-        <v>642</v>
+        <v>626</v>
       </c>
       <c r="C180" t="s">
-        <v>643</v>
+        <v>627</v>
       </c>
       <c r="D180" t="s">
-        <v>644</v>
+        <v>628</v>
+      </c>
+      <c r="E180" t="s">
+        <v>206</v>
+      </c>
+      <c r="F180" t="s">
+        <v>629</v>
       </c>
     </row>
     <row r="181" spans="1:6">
       <c r="A181" t="s">
-        <v>645</v>
+        <v>630</v>
       </c>
       <c r="B181" t="s">
-        <v>646</v>
-      </c>
-      <c r="C181" t="s">
-        <v>646</v>
-      </c>
-      <c r="D181" t="s">
-        <v>647</v>
+        <v>631</v>
       </c>
       <c r="E181" t="s">
-        <v>648</v>
+        <v>41</v>
       </c>
       <c r="F181" t="s">
-        <v>649</v>
+        <v>632</v>
       </c>
     </row>
     <row r="182" spans="1:6">
       <c r="A182" t="s">
-        <v>650</v>
+        <v>633</v>
       </c>
       <c r="B182" t="s">
-        <v>651</v>
-      </c>
-      <c r="C182" t="s">
-        <v>652</v>
-      </c>
-      <c r="D182" t="s">
-        <v>651</v>
+        <v>634</v>
       </c>
       <c r="E182" t="s">
-        <v>228</v>
-      </c>
-      <c r="F182" t="s">
-        <v>653</v>
+        <v>41</v>
       </c>
     </row>
     <row r="183" spans="1:6">
       <c r="A183" t="s">
-        <v>654</v>
+        <v>635</v>
       </c>
       <c r="B183" t="s">
-        <v>655</v>
-      </c>
-      <c r="C183" t="s">
-        <v>656</v>
-      </c>
-      <c r="D183" t="s">
-        <v>655</v>
+        <v>636</v>
       </c>
       <c r="E183" t="s">
-        <v>657</v>
+        <v>41</v>
       </c>
       <c r="F183" t="s">
-        <v>658</v>
+        <v>637</v>
       </c>
     </row>
     <row r="184" spans="1:6">
       <c r="A184" t="s">
-        <v>659</v>
+        <v>638</v>
       </c>
       <c r="B184" t="s">
-        <v>660</v>
-      </c>
-      <c r="C184" t="s">
-        <v>661</v>
-      </c>
-      <c r="D184" t="s">
-        <v>660</v>
+        <v>639</v>
       </c>
       <c r="E184" t="s">
-        <v>152</v>
+        <v>41</v>
       </c>
       <c r="F184" t="s">
-        <v>662</v>
+        <v>640</v>
       </c>
     </row>
     <row r="185" spans="1:6">
       <c r="A185" t="s">
-        <v>663</v>
+        <v>641</v>
       </c>
       <c r="B185" t="s">
-        <v>664</v>
-      </c>
-      <c r="E185" t="s">
-        <v>665</v>
-      </c>
-      <c r="F185" t="s">
-        <v>666</v>
+        <v>642</v>
+      </c>
+      <c r="C185" t="s">
+        <v>643</v>
+      </c>
+      <c r="D185" t="s">
+        <v>644</v>
       </c>
     </row>
     <row r="186" spans="1:6">
       <c r="A186" t="s">
-        <v>667</v>
+        <v>645</v>
       </c>
       <c r="B186" t="s">
-        <v>668</v>
+        <v>646</v>
+      </c>
+      <c r="C186" t="s">
+        <v>646</v>
+      </c>
+      <c r="D186" t="s">
+        <v>647</v>
       </c>
       <c r="E186" t="s">
-        <v>349</v>
-      </c>
-      <c r="F186">
-        <v>12374842</v>
+        <v>648</v>
+      </c>
+      <c r="F186" t="s">
+        <v>649</v>
       </c>
     </row>
     <row r="187" spans="1:6">
       <c r="A187" t="s">
-        <v>669</v>
+        <v>650</v>
       </c>
       <c r="B187" t="s">
-        <v>670</v>
+        <v>651</v>
       </c>
       <c r="C187" t="s">
-        <v>670</v>
+        <v>652</v>
       </c>
       <c r="D187" t="s">
-        <v>671</v>
+        <v>651</v>
       </c>
       <c r="E187" t="s">
-        <v>349</v>
+        <v>228</v>
       </c>
       <c r="F187" t="s">
-        <v>672</v>
+        <v>653</v>
       </c>
     </row>
     <row r="188" spans="1:6">
       <c r="A188" t="s">
-        <v>673</v>
+        <v>654</v>
       </c>
       <c r="B188" t="s">
-        <v>674</v>
+        <v>655</v>
       </c>
       <c r="C188" t="s">
-        <v>675</v>
+        <v>656</v>
+      </c>
+      <c r="D188" t="s">
+        <v>655</v>
       </c>
       <c r="E188" t="s">
-        <v>75</v>
+        <v>657</v>
       </c>
       <c r="F188" t="s">
-        <v>676</v>
+        <v>658</v>
       </c>
     </row>
     <row r="189" spans="1:6">
       <c r="A189" t="s">
-        <v>677</v>
+        <v>659</v>
       </c>
       <c r="B189" t="s">
-        <v>678</v>
+        <v>660</v>
       </c>
       <c r="C189" t="s">
-        <v>679</v>
+        <v>661</v>
       </c>
       <c r="D189" t="s">
-        <v>678</v>
+        <v>660</v>
       </c>
       <c r="E189" t="s">
-        <v>16</v>
-      </c>
-      <c r="F189">
-        <v>9371449</v>
+        <v>152</v>
+      </c>
+      <c r="F189" t="s">
+        <v>662</v>
       </c>
     </row>
     <row r="190" spans="1:6">
       <c r="A190" t="s">
-        <v>680</v>
+        <v>663</v>
       </c>
       <c r="B190" t="s">
-        <v>681</v>
+        <v>664</v>
       </c>
       <c r="E190" t="s">
-        <v>5</v>
+        <v>665</v>
       </c>
       <c r="F190" t="s">
-        <v>682</v>
+        <v>666</v>
       </c>
     </row>
     <row r="191" spans="1:6">
       <c r="A191" t="s">
-        <v>683</v>
+        <v>667</v>
       </c>
       <c r="B191" t="s">
-        <v>684</v>
+        <v>668</v>
       </c>
       <c r="E191" t="s">
-        <v>23</v>
-      </c>
-      <c r="F191" t="s">
-        <v>685</v>
+        <v>349</v>
+      </c>
+      <c r="F191">
+        <v>12374842</v>
       </c>
     </row>
     <row r="192" spans="1:6">
       <c r="A192" t="s">
-        <v>686</v>
+        <v>669</v>
       </c>
       <c r="B192" t="s">
-        <v>687</v>
+        <v>670</v>
+      </c>
+      <c r="C192" t="s">
+        <v>670</v>
+      </c>
+      <c r="D192" t="s">
+        <v>671</v>
       </c>
       <c r="E192" t="s">
-        <v>251</v>
-      </c>
-      <c r="F192">
-        <v>17170003</v>
+        <v>349</v>
+      </c>
+      <c r="F192" t="s">
+        <v>672</v>
       </c>
     </row>
     <row r="193" spans="1:6">
       <c r="A193" t="s">
-        <v>688</v>
+        <v>673</v>
       </c>
       <c r="B193" t="s">
-        <v>689</v>
+        <v>674</v>
+      </c>
+      <c r="C193" t="s">
+        <v>675</v>
       </c>
       <c r="E193" t="s">
-        <v>251</v>
-      </c>
-      <c r="F193">
-        <v>17170003</v>
+        <v>75</v>
+      </c>
+      <c r="F193" t="s">
+        <v>676</v>
       </c>
     </row>
     <row r="194" spans="1:6">
       <c r="A194" t="s">
-        <v>690</v>
+        <v>677</v>
       </c>
       <c r="B194" t="s">
-        <v>691</v>
+        <v>678</v>
+      </c>
+      <c r="C194" t="s">
+        <v>679</v>
+      </c>
+      <c r="D194" t="s">
+        <v>678</v>
       </c>
       <c r="E194" t="s">
-        <v>692</v>
+        <v>16</v>
       </c>
       <c r="F194">
-        <v>22685278</v>
+        <v>9371449</v>
       </c>
     </row>
     <row r="195" spans="1:6">
       <c r="A195" t="s">
-        <v>693</v>
+        <v>680</v>
       </c>
       <c r="B195" t="s">
-        <v>694</v>
+        <v>681</v>
       </c>
       <c r="E195" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F195" t="s">
-        <v>695</v>
+        <v>682</v>
       </c>
     </row>
     <row r="196" spans="1:6">
       <c r="A196" t="s">
-        <v>696</v>
+        <v>683</v>
       </c>
       <c r="B196" t="s">
-        <v>697</v>
+        <v>684</v>
       </c>
       <c r="E196" t="s">
-        <v>698</v>
-      </c>
-      <c r="F196">
-        <v>18309357</v>
+        <v>23</v>
+      </c>
+      <c r="F196" t="s">
+        <v>685</v>
       </c>
     </row>
     <row r="197" spans="1:6">
       <c r="A197" t="s">
-        <v>699</v>
+        <v>686</v>
       </c>
       <c r="B197" t="s">
-        <v>700</v>
+        <v>687</v>
       </c>
       <c r="E197" t="s">
-        <v>701</v>
-      </c>
-      <c r="F197" t="s">
-        <v>702</v>
+        <v>251</v>
+      </c>
+      <c r="F197">
+        <v>17170003</v>
       </c>
     </row>
     <row r="198" spans="1:6">
       <c r="A198" t="s">
-        <v>703</v>
+        <v>688</v>
       </c>
       <c r="B198" t="s">
-        <v>704</v>
-      </c>
-      <c r="E198" t="s">
-        <v>705</v>
-      </c>
-      <c r="F198">
-        <v>23222720</v>
+        <v>735</v>
       </c>
     </row>
     <row r="199" spans="1:6">
       <c r="A199" t="s">
-        <v>706</v>
+        <v>688</v>
       </c>
       <c r="B199" t="s">
-        <v>707</v>
+        <v>689</v>
       </c>
       <c r="E199" t="s">
-        <v>23</v>
-      </c>
-      <c r="F199" t="s">
-        <v>708</v>
+        <v>251</v>
+      </c>
+      <c r="F199">
+        <v>17170003</v>
       </c>
     </row>
     <row r="200" spans="1:6">
       <c r="A200" t="s">
-        <v>709</v>
+        <v>690</v>
       </c>
       <c r="B200" t="s">
-        <v>710</v>
-      </c>
-      <c r="C200" t="s">
-        <v>710</v>
-      </c>
-      <c r="D200" t="s">
-        <v>711</v>
+        <v>691</v>
+      </c>
+      <c r="E200" t="s">
+        <v>692</v>
+      </c>
+      <c r="F200">
+        <v>22685278</v>
       </c>
     </row>
     <row r="201" spans="1:6">
       <c r="A201" t="s">
-        <v>712</v>
+        <v>693</v>
       </c>
       <c r="B201" t="s">
-        <v>713</v>
-      </c>
-      <c r="C201" t="s">
-        <v>714</v>
-      </c>
-      <c r="D201" t="s">
-        <v>713</v>
+        <v>694</v>
       </c>
       <c r="E201" t="s">
-        <v>290</v>
+        <v>13</v>
       </c>
       <c r="F201" t="s">
-        <v>715</v>
+        <v>695</v>
       </c>
     </row>
     <row r="202" spans="1:6">
       <c r="A202" t="s">
-        <v>716</v>
+        <v>696</v>
       </c>
       <c r="B202" t="s">
-        <v>717</v>
-      </c>
-      <c r="C202" t="s">
-        <v>718</v>
-      </c>
-      <c r="D202" t="s">
-        <v>717</v>
+        <v>697</v>
       </c>
       <c r="E202" t="s">
-        <v>719</v>
+        <v>698</v>
       </c>
       <c r="F202">
-        <v>11243806</v>
+        <v>18309357</v>
       </c>
     </row>
     <row r="203" spans="1:6">
       <c r="A203" t="s">
+        <v>699</v>
+      </c>
+      <c r="B203" t="s">
+        <v>700</v>
+      </c>
+      <c r="E203" t="s">
+        <v>701</v>
+      </c>
+      <c r="F203" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6">
+      <c r="A204" t="s">
+        <v>703</v>
+      </c>
+      <c r="B204" t="s">
+        <v>704</v>
+      </c>
+      <c r="E204" t="s">
+        <v>705</v>
+      </c>
+      <c r="F204">
+        <v>23222720</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6">
+      <c r="A205" t="s">
+        <v>706</v>
+      </c>
+      <c r="B205" t="s">
+        <v>707</v>
+      </c>
+      <c r="E205" t="s">
+        <v>23</v>
+      </c>
+      <c r="F205" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6">
+      <c r="A206" t="s">
+        <v>709</v>
+      </c>
+      <c r="B206" t="s">
+        <v>710</v>
+      </c>
+      <c r="C206" t="s">
+        <v>710</v>
+      </c>
+      <c r="D206" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6">
+      <c r="A207" t="s">
+        <v>712</v>
+      </c>
+      <c r="B207" t="s">
+        <v>713</v>
+      </c>
+      <c r="C207" t="s">
+        <v>714</v>
+      </c>
+      <c r="D207" t="s">
+        <v>713</v>
+      </c>
+      <c r="E207" t="s">
+        <v>290</v>
+      </c>
+      <c r="F207" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6">
+      <c r="A208" t="s">
+        <v>716</v>
+      </c>
+      <c r="B208" t="s">
+        <v>717</v>
+      </c>
+      <c r="C208" t="s">
+        <v>718</v>
+      </c>
+      <c r="D208" t="s">
+        <v>717</v>
+      </c>
+      <c r="E208" t="s">
+        <v>719</v>
+      </c>
+      <c r="F208">
+        <v>11243806</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6">
+      <c r="A209" t="s">
         <v>720</v>
       </c>
-      <c r="B203" t="s">
+      <c r="B209" t="s">
         <v>721</v>
       </c>
-      <c r="C203" t="s">
+      <c r="C209" t="s">
         <v>722</v>
       </c>
-      <c r="D203" t="s">
+      <c r="D209" t="s">
         <v>721</v>
       </c>
-      <c r="E203" t="s">
+      <c r="E209" t="s">
         <v>152</v>
       </c>
-      <c r="F203" t="s">
+      <c r="F209" t="s">
         <v>723</v>
       </c>
     </row>

</xml_diff>